<commit_message>
feat: add description to rfc form
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/referral_for_care.xlsx
+++ b/config/itech-aurum/forms/app/referral_for_care.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/femioni/medic/config-itech/itech-aurum/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E34F3A1-969E-2649-B3B7-DBAB2F24D30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19A83EF-8690-8043-B79D-DB74D39440AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-2900" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="94">
   <si>
     <t>type</t>
   </si>
@@ -176,9 +176,6 @@
     <t>Specify other</t>
   </si>
   <si>
-    <t>selected(${symptoms_list}, 'other')</t>
-  </si>
-  <si>
     <t>additional_notes</t>
   </si>
   <si>
@@ -279,6 +276,39 @@
   </si>
   <si>
     <t>instance::tag</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>NO_LABEL</t>
+  </si>
+  <si>
+    <t>instructions</t>
+  </si>
+  <si>
+    <t>Referral for Care Form: Used by the super nurse or site Nurse to refer Clients to the Clinic for attention. Submitting this form triggers the Client Review: Potential AE task which can be accessed by either the hub or the site nurse. This task form should also be accessible as an Action in the client profile.</t>
+  </si>
+  <si>
+    <t>form</t>
+  </si>
+  <si>
+    <t>../form/symptoms_list</t>
+  </si>
+  <si>
+    <t>../form/additional_notes</t>
+  </si>
+  <si>
+    <t>selected(../symptoms_list, 'other')</t>
+  </si>
+  <si>
+    <t>../form/symptoms_other</t>
+  </si>
+  <si>
+    <t>selected(../form/symptoms_list, 'other')</t>
+  </si>
+  <si>
+    <t>h4 blue</t>
   </si>
 </sst>
 </file>
@@ -288,7 +318,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -369,6 +399,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -418,9 +460,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+  <cellXfs count="25">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -430,7 +472,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -440,38 +482,38 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,11 +729,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z992"/>
+  <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L27" sqref="L27"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -703,10 +745,12 @@
     <col min="5" max="5" width="9.33203125" customWidth="1"/>
     <col min="6" max="7" width="11.5" customWidth="1"/>
     <col min="8" max="8" width="34" customWidth="1"/>
-    <col min="9" max="26" width="11.5" customWidth="1"/>
+    <col min="9" max="10" width="11.5" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" customWidth="1"/>
+    <col min="12" max="26" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -742,7 +786,7 @@
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -883,75 +927,75 @@
       <c r="A11" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14" t="s">
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="14"/>
-      <c r="T11" s="14"/>
-      <c r="U11" s="14"/>
-      <c r="V11" s="14"/>
-      <c r="W11" s="14"/>
-      <c r="X11" s="14"/>
-      <c r="Y11" s="14"/>
-      <c r="Z11" s="14"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="12"/>
+      <c r="X11" s="12"/>
+      <c r="Y11" s="12"/>
+      <c r="Z11" s="12"/>
     </row>
     <row r="12" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="14" t="s">
         <v>39</v>
       </c>
       <c r="E12" s="10"/>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="14" t="s">
         <v>29</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="16" t="s">
+      <c r="J12" s="12"/>
+      <c r="K12" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="L12" s="14"/>
+      <c r="L12" s="12"/>
       <c r="M12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="14"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="14"/>
-      <c r="U12" s="14"/>
-      <c r="V12" s="14"/>
-      <c r="W12" s="14"/>
-      <c r="X12" s="14"/>
-      <c r="Y12" s="14"/>
-      <c r="Z12" s="14"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="12"/>
+      <c r="W12" s="12"/>
+      <c r="X12" s="12"/>
+      <c r="Y12" s="12"/>
+      <c r="Z12" s="12"/>
     </row>
     <row r="13" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
@@ -960,7 +1004,7 @@
       <c r="B13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="15" t="s">
         <v>41</v>
       </c>
       <c r="D13" s="5"/>
@@ -989,132 +1033,222 @@
       <c r="Y13" s="5"/>
       <c r="Z13" s="5"/>
     </row>
-    <row r="14" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
-      <c r="V14" s="18"/>
-      <c r="W14" s="18"/>
-      <c r="X14" s="18"/>
-      <c r="Y14" s="18"/>
-      <c r="Z14" s="18"/>
+    <row r="14" spans="1:26" ht="119" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="5"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="5"/>
     </row>
     <row r="15" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="5"/>
-      <c r="U15" s="5"/>
-      <c r="V15" s="5"/>
-      <c r="W15" s="5"/>
-      <c r="X15" s="5"/>
-      <c r="Y15" s="5"/>
-      <c r="Z15" s="5"/>
+      <c r="A15" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="5"/>
+      <c r="V16" s="5"/>
+      <c r="W16" s="5"/>
+      <c r="X16" s="5"/>
+      <c r="Y16" s="5"/>
+      <c r="Z16" s="5"/>
+    </row>
+    <row r="17" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B17" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="5"/>
+      <c r="Z17" s="5"/>
+    </row>
+    <row r="18" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="18"/>
-      <c r="T16" s="18"/>
-      <c r="U16" s="18"/>
-      <c r="V16" s="18"/>
-      <c r="W16" s="18"/>
-      <c r="X16" s="18"/>
-      <c r="Y16" s="18"/>
-      <c r="Z16" s="18"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="5"/>
+      <c r="W18" s="5"/>
+      <c r="X18" s="5"/>
+      <c r="Y18" s="5"/>
+      <c r="Z18" s="5"/>
     </row>
-    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="K20" s="23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="K21" s="23" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="K22" s="23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2075,6 +2209,8 @@
     <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -2101,7 +2237,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -2116,80 +2252,80 @@
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="C3" s="11" t="s">
         <v>55</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="19" t="s">
+      <c r="A4" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>57</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="19" t="s">
+      <c r="A5" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>59</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" s="19" t="s">
+      <c r="A6" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>61</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" s="19" t="s">
+      <c r="A7" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>63</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="19" t="s">
+      <c r="A8" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>65</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="19" t="s">
+      <c r="A9" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>67</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2231,7 +2367,7 @@
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
-      <c r="C18" s="21"/>
+      <c r="C18" s="17"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3218,94 +3354,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="C1" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="D1" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="E1" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="F1" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="G1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="G1" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="22" t="s">
+      <c r="I1" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
+      <c r="Y1" s="19"/>
+      <c r="Z1" s="19"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="C2" s="21">
+        <v>43896</v>
+      </c>
+      <c r="D2" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="26">
-        <v>43896</v>
-      </c>
-      <c r="D2" s="25" t="s">
+      <c r="E2" t="s">
         <v>79</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="G2" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25" t="s">
+      <c r="H2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I2" t="s">
         <v>81</v>
       </c>
-      <c r="H2" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
-      <c r="T2" s="25"/>
-      <c r="U2" s="25"/>
-      <c r="V2" s="25"/>
-      <c r="W2" s="25"/>
-      <c r="X2" s="25"/>
-      <c r="Y2" s="25"/>
-      <c r="Z2" s="25"/>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>